<commit_message>
CAGRID-864: 1.5 known issues and release notes
</commit_message>
<xml_diff>
--- a/cagrid/Documentation/core/release_notes/1.5/caGrid 1.5 known issues.xlsx
+++ b/cagrid/Documentation/core/release_notes/1.5/caGrid 1.5 known issues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="580" windowWidth="20820" windowHeight="12980" tabRatio="500"/>
+    <workbookView xWindow="-26180" yWindow="4020" windowWidth="20820" windowHeight="12980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="general_report" sheetId="2" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -568,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>